<commit_message>
oprava procesoru pro start a restart
</commit_message>
<xml_diff>
--- a/Dokumentace/Tla��tka decoder.xlsx
+++ b/Dokumentace/Tla��tka decoder.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="28755" windowHeight="12330"/>
@@ -11,7 +11,7 @@
     <sheet name="List2" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -155,11 +155,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,15 +236,20 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv sady Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -318,6 +323,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -352,6 +358,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kancelář">
@@ -527,21 +534,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="18">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -561,7 +568,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -585,7 +592,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -609,7 +616,7 @@
         <v>11110.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -633,7 +640,7 @@
         <v>11101.1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +664,7 @@
         <v>11100.1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -681,7 +688,7 @@
         <v>11011.1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -705,7 +712,7 @@
         <v>11010.1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -729,7 +736,7 @@
         <v>11001.1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -753,7 +760,7 @@
         <v>11000.011</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -777,7 +784,7 @@
         <v>10111.011</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -801,7 +808,7 @@
         <v>10110.1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -825,7 +832,7 @@
         <v>10101.1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -849,7 +856,7 @@
         <v>10100.1</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -873,7 +880,7 @@
         <v>10011.011</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -897,7 +904,7 @@
         <v>10010.1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -921,7 +928,7 @@
         <v>10001.1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -945,7 +952,7 @@
         <v>10000.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -976,24 +983,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>